<commit_message>
Added printer class and other changes
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\H1\ObjektOrienteretProgrammering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E920511-2F9B-4646-B36D-19BFB183DD17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6063B2C1-CE84-4E8D-BCC3-7FDCA8B35894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5A37C7E3-6A95-4FF6-ACBB-059AB5A0E1D3}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" xr2:uid="{5A37C7E3-6A95-4FF6-ACBB-059AB5A0E1D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -159,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,6 +203,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,6 +656,69 @@
             <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>+----+----+----+----+----+----+</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>|    |    |    |    |    |    |</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>|    |    |    |    |    |    |</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>+----+----+----+----+----+----+</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>|    |</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>|    |</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="2400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>+----+</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -947,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE11885-2A2B-4472-9901-EE7C900043CA}">
-  <dimension ref="B2:AR15"/>
+  <dimension ref="A1:AR24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -958,7 +1035,57 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="B2" s="2">
         <v>44</v>
       </c>
@@ -1063,7 +1190,10 @@
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
     </row>
-    <row r="3" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="B3" s="4">
         <v>43</v>
       </c>
@@ -1080,7 +1210,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
       <c r="B4" s="2">
         <v>42</v>
       </c>
@@ -1097,7 +1230,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
       <c r="B5" s="4">
         <v>41</v>
       </c>
@@ -1114,7 +1250,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
       <c r="B6" s="2">
         <v>40</v>
       </c>
@@ -1131,7 +1270,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
       <c r="B7" s="11">
         <v>39</v>
       </c>
@@ -1148,7 +1290,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
       <c r="B8" s="2">
         <v>38</v>
       </c>
@@ -1183,7 +1328,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
       <c r="B9" s="2">
         <v>37</v>
       </c>
@@ -1218,7 +1366,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
       <c r="B10" s="2">
         <v>36</v>
       </c>
@@ -1235,7 +1386,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
       <c r="B11" s="2">
         <v>35</v>
       </c>
@@ -1252,7 +1406,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
       <c r="B12" s="2">
         <v>34</v>
       </c>
@@ -1314,7 +1471,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
       <c r="B13" s="2">
         <v>33</v>
       </c>
@@ -1325,7 +1485,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
       <c r="B14" s="2">
         <v>32</v>
       </c>
@@ -1336,7 +1499,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
       <c r="B15" s="2">
         <v>31</v>
       </c>
@@ -1378,6 +1544,261 @@
       </c>
       <c r="O15" s="2">
         <v>18</v>
+      </c>
+      <c r="R15" s="2">
+        <v>42</v>
+      </c>
+      <c r="S15" s="6">
+        <v>43</v>
+      </c>
+      <c r="T15" s="2">
+        <v>44</v>
+      </c>
+      <c r="U15" s="2">
+        <v>45</v>
+      </c>
+      <c r="V15" s="2">
+        <v>46</v>
+      </c>
+      <c r="W15" s="2">
+        <v>47</v>
+      </c>
+      <c r="X15" s="2">
+        <v>48</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>49</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>50</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>51</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH15" s="5">
+        <v>6</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y16" s="7">
+        <v>52</v>
+      </c>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>53</v>
+      </c>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y18" s="7">
+        <v>54</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>69</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>63</v>
+      </c>
+      <c r="AD18" s="9">
+        <v>62</v>
+      </c>
+      <c r="AE18" s="9">
+        <v>61</v>
+      </c>
+      <c r="AF18" s="9">
+        <v>60</v>
+      </c>
+      <c r="AG18" s="9">
+        <v>59</v>
+      </c>
+      <c r="AH18" s="9">
+        <v>58</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y19" s="7">
+        <v>55</v>
+      </c>
+      <c r="AB19" s="10">
+        <v>68</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R20" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y20" s="7">
+        <v>56</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>67</v>
+      </c>
+      <c r="AH20" s="12"/>
+      <c r="AI20" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="2">
+        <v>36</v>
+      </c>
+      <c r="S21" s="11">
+        <v>70</v>
+      </c>
+      <c r="T21" s="11">
+        <v>71</v>
+      </c>
+      <c r="U21" s="11">
+        <v>72</v>
+      </c>
+      <c r="V21" s="11">
+        <v>73</v>
+      </c>
+      <c r="W21" s="11">
+        <v>74</v>
+      </c>
+      <c r="X21" s="11">
+        <v>75</v>
+      </c>
+      <c r="Y21" s="8">
+        <v>57</v>
+      </c>
+      <c r="AB21" s="10">
+        <v>66</v>
+      </c>
+      <c r="AH21" s="12"/>
+      <c r="AI21" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB22" s="10">
+        <v>65</v>
+      </c>
+      <c r="AH22" s="12"/>
+      <c r="AI22" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>64</v>
+      </c>
+      <c r="AH23" s="12"/>
+      <c r="AI23" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="18:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="2">
+        <v>33</v>
+      </c>
+      <c r="S24" s="6">
+        <v>32</v>
+      </c>
+      <c r="T24" s="2">
+        <v>31</v>
+      </c>
+      <c r="U24" s="2">
+        <v>30</v>
+      </c>
+      <c r="V24" s="2">
+        <v>29</v>
+      </c>
+      <c r="W24" s="2">
+        <v>28</v>
+      </c>
+      <c r="X24" s="2">
+        <v>27</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>26</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>25</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>24</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>23</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>22</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>21</v>
+      </c>
+      <c r="AE24" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF24" s="2">
+        <v>19</v>
+      </c>
+      <c r="AG24" s="2">
+        <v>18</v>
+      </c>
+      <c r="AH24" s="4">
+        <v>17</v>
+      </c>
+      <c r="AI24" s="2">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a lot of features
Overtake functions, better user experience, pretty end screen, added aI
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\H1\ObjektOrienteretProgrammering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6063B2C1-CE84-4E8D-BCC3-7FDCA8B35894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B8B2FA-2AAE-4BB2-B70D-670331154A3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" xr2:uid="{5A37C7E3-6A95-4FF6-ACBB-059AB5A0E1D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5A37C7E3-6A95-4FF6-ACBB-059AB5A0E1D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1030,7 @@
   <dimension ref="A1:AR24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1220,6 +1223,9 @@
       <c r="H4" s="7">
         <v>53</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="O4" s="2">
         <v>7</v>
       </c>
@@ -1277,6 +1283,9 @@
       <c r="B7" s="11">
         <v>39</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H7" s="7">
         <v>56</v>
       </c>
@@ -1376,6 +1385,9 @@
       <c r="I10" s="10">
         <v>68</v>
       </c>
+      <c r="M10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="O10" s="9">
         <v>13</v>
       </c>
@@ -1477,6 +1489,9 @@
       </c>
       <c r="B13" s="2">
         <v>33</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="I13" s="10">
         <v>65</v>

</xml_diff>